<commit_message>
Updated instructions and parts list
</commit_message>
<xml_diff>
--- a/Solar Charger 2017 PCB/SolarCharger2017.xlsx
+++ b/Solar Charger 2017 PCB/SolarCharger2017.xlsx
@@ -12,6 +12,7 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">SolarCharger2017!$A$1:$H$30</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">SolarCharger2017!$A$1:$H$30</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -73,6 +74,141 @@
     <t xml:space="preserve">http://www.ebay.co.uk/itm/122466718109</t>
   </si>
   <si>
+    <t xml:space="preserve">C1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1uF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">matts_components:C1V7_lg_pad_lg_hole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REInnovationFootprint:TH_LED-5MM_larg_pad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DCDC1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DC-DC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REInnovationFootprint:TH_DCDC_Converter_USB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aliexpress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DCDC2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REInnovationFootprint:TH_DCDC_Converter_NoUSB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LG1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOGO1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CuriousElectric3:CEC_Globe_10mm_FCU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LG2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOGO2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CuriousElectric3:TCEC_Words_13mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5V OUT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REInnovationFootprint:SIL-2_screw_terminal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LiIon Cell V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REInnovationFootprint:SIL_2_screw_+_JST_2mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PV IN 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PV IN 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCB1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REInnovationFootprint:PCB_65x90mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elecrow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REInnovationFootprint:TH_Resistor_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.2k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R4</t>
+  </si>
+  <si>
     <t xml:space="preserve">SC1</t>
   </si>
   <si>
@@ -85,16 +221,13 @@
     <t xml:space="preserve">1-2W solar PV module</t>
   </si>
   <si>
-    <t xml:space="preserve">Aliexpress</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DCDC1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DC-DC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REInnovationFootprint:TH_DCDC_Converter_USB</t>
+    <t xml:space="preserve">SW1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5V ON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REInnovationFootprint:SW_SPDT_R_Angle_ALIEX</t>
   </si>
   <si>
     <t xml:space="preserve">U1</t>
@@ -119,138 +252,6 @@
   </si>
   <si>
     <t xml:space="preserve">Texas Instruments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REInnovationFootprint:TH_LED-5MM_larg_pad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.2k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REInnovationFootprint:TH_Resistor_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1uF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">matts_components:C1V7_lg_pad_lg_hole</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LiIon Cell V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REInnovationFootprint:SIL_2_screw_+_JST_2mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SW1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5V ON</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REInnovationFootprint:SW_SPDT_R_Angle_ALIEX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LG1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOGO1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CuriousElectric3:CEC_Globe_10mm_FCU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LG2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOGO2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CuriousElectric3:TCEC_Words_13mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5V OUT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REInnovationFootprint:SIL-2_screw_terminal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PV IN 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PV IN 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PCB1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PCB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REInnovationFootprint:PCB_65x90mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Elecrow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DCDC2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REInnovationFootprint:TH_DCDC_Converter_NoUSB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P5</t>
   </si>
   <si>
     <t xml:space="preserve">Hardware</t>
@@ -392,7 +393,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D31" activeCellId="0" sqref="D31"/>
+      <selection pane="bottomRight" activeCell="A2" activeCellId="0" sqref="A2:B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -475,74 +476,47 @@
       <c r="C3" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>20</v>
-      </c>
       <c r="H3" s="0" t="n">
-        <v>2.5</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H4" s="0" t="n">
-        <v>1.5</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="H5" s="0" t="n">
-        <v>2.88</v>
-      </c>
-      <c r="I5" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="J5" s="0" t="s">
-        <v>25</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="H6" s="0" t="n">
         <v>0.05</v>
@@ -550,239 +524,266 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>34</v>
+        <v>27</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>28</v>
       </c>
       <c r="H7" s="0" t="n">
-        <v>0.05</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>39</v>
+        <v>30</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>28</v>
       </c>
       <c r="H8" s="0" t="n">
-        <v>0.01</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="H9" s="0" t="n">
-        <v>0.01</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="H10" s="0" t="n">
-        <v>0.1</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="H11" s="0" t="n">
-        <v>0.1</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="H12" s="0" t="n">
-        <v>0.01</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H14" s="0" t="n">
-        <v>0.2</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="H15" s="0" t="n">
-        <v>0.01</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>60</v>
+        <v>51</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>63</v>
+        <v>55</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <v>0.01</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>49</v>
+        <v>55</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <v>0.01</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>49</v>
+        <v>55</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>0.01</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="F21" s="0" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="H21" s="0" t="n">
-        <v>3</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>73</v>
+        <v>63</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>64</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="H22" s="0" t="n">
-        <v>1</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="H23" s="0" t="n">
+        <v>0.2</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="H24" s="0" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="I24" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="B24" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>49</v>
+      <c r="J24" s="0" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>